<commit_message>
update of upset and donut plot code
</commit_message>
<xml_diff>
--- a/output/Stats/stats.xlsx
+++ b/output/Stats/stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remi.gschwind\Desktop\Resfinder FG\ResFinder_FG_Analysis\ResFinder_FG_Analysis\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remi.gschwind\Desktop\Resfinder FG\ResFinder_FG_Analysis\ResFinder_FG_Analysis\output\Stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B03A56-C35E-4A2B-93EB-1C6080CB2732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BB72EA-BE21-48F7-A5AB-D8FA720D9C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ABC25C7F-699F-4522-8C96-2753F7B0DD00}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{ABC25C7F-699F-4522-8C96-2753F7B0DD00}"/>
   </bookViews>
   <sheets>
     <sheet name="Hits_spe" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="59">
   <si>
     <t>n gene</t>
   </si>
@@ -209,6 +209,12 @@
   </si>
   <si>
     <t>aminocoumarin</t>
+  </si>
+  <si>
+    <t>proportion</t>
+  </si>
+  <si>
+    <t>propotion</t>
   </si>
 </sst>
 </file>
@@ -570,7 +576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF7D0970-32F0-4CF7-B959-659B9EBEEE3A}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -1127,23 +1133,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{520A1805-9242-48BA-952D-546C1C8D119F}">
-  <dimension ref="A1:R25"/>
+  <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1"/>
     <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14" customWidth="1"/>
+    <col min="20" max="20" width="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>46</v>
       </c>
@@ -1154,49 +1165,64 @@
         <v>47</v>
       </c>
       <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>50</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" t="s">
         <v>51</v>
-      </c>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N1" t="s">
-        <v>53</v>
       </c>
       <c r="O1" t="s">
         <v>16</v>
       </c>
       <c r="P1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>57</v>
+      </c>
+      <c r="R1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="U1" t="s">
+        <v>58</v>
+      </c>
+      <c r="V1" t="s">
         <v>54</v>
       </c>
-      <c r="R1" t="s">
+      <c r="W1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1209,55 +1235,75 @@
       <c r="D2">
         <v>160</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
+        <f>D2/$D$24*100</f>
+        <v>5.2892561983471076</v>
+      </c>
+      <c r="F2">
         <v>121</v>
       </c>
-      <c r="F2" s="2">
-        <f>E2/$B2*100</f>
+      <c r="G2" s="2">
+        <f>F2/$B2*100</f>
         <v>23.224568138195778</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>348</v>
       </c>
-      <c r="H2">
+      <c r="I2" s="2">
+        <f>H2/$H$24*100</f>
+        <v>8.2817705854355061</v>
+      </c>
+      <c r="J2">
         <v>227</v>
       </c>
-      <c r="I2" s="2">
-        <f>H2/$B2*100</f>
+      <c r="K2" s="2">
+        <f>J2/$B2*100</f>
         <v>43.570057581573899</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>123</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2">
-        <f>K2/$B2*100</f>
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>148</v>
+      <c r="M2" s="2">
+        <f>L2/$L$24*100</f>
+        <v>11.191992720655142</v>
       </c>
       <c r="N2">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="O2" s="2">
         <f>N2/$B2*100</f>
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>148</v>
+      </c>
+      <c r="Q2" s="2">
+        <f>P2/$P$24*100</f>
+        <v>10.938654841093866</v>
+      </c>
+      <c r="R2">
+        <v>22</v>
+      </c>
+      <c r="S2" s="2">
+        <f>R2/$B2*100</f>
         <v>4.2226487523992322</v>
       </c>
-      <c r="P2">
+      <c r="T2">
         <v>139</v>
       </c>
-      <c r="Q2">
+      <c r="U2" s="2">
+        <f>T2/$T$24*100</f>
+        <v>10.404191616766468</v>
+      </c>
+      <c r="V2">
         <v>5</v>
       </c>
-      <c r="R2" s="2">
-        <f>Q2/$B2*100</f>
+      <c r="W2" s="2">
+        <f>V2/$B2*100</f>
         <v>0.95969289827255266</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1270,55 +1316,75 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <f t="shared" ref="F3:F24" si="0">E3/$B3*100</f>
-        <v>0</v>
-      </c>
-      <c r="G3">
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E24" si="0">D3/$D$24*100</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G24" si="1">F3/$B3*100</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I24" si="1">H3/$B3*100</f>
-        <v>0</v>
+        <f t="shared" ref="I3:I24" si="2">H3/$H$24*100</f>
+        <v>2.3798191337458353E-2</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="2">
-        <f t="shared" ref="L3:L24" si="2">K3/$B3*100</f>
-        <v>0</v>
-      </c>
-      <c r="M3">
+      <c r="K3" s="2">
+        <f t="shared" ref="K3:K24" si="3">J3/$B3*100</f>
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <f t="shared" ref="M3:M24" si="4">L3/$L$24*100</f>
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
+        <f t="shared" ref="O3:O24" si="5">N3/$B3*100</f>
+        <v>0</v>
+      </c>
+      <c r="P3">
         <v>1</v>
       </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3" s="2">
-        <f t="shared" ref="O3:O24" si="3">N3/$B3*100</f>
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3" s="2">
-        <f t="shared" ref="R3:R24" si="4">Q3/$B3*100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q3" s="2">
+        <f t="shared" ref="Q3:Q24" si="6">P3/$P$24*100</f>
+        <v>7.3909830007390986E-2</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3" s="2">
+        <f t="shared" ref="S3:S24" si="7">R3/$B3*100</f>
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3" s="2">
+        <f t="shared" ref="U3:U24" si="8">T3/$T$24*100</f>
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3" s="2">
+        <f t="shared" ref="W3:W24" si="9">V3/$B3*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1331,55 +1397,75 @@
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="E4" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>20</v>
       </c>
-      <c r="H4">
+      <c r="I4" s="2">
+        <f t="shared" si="2"/>
+        <v>0.47596382674916704</v>
+      </c>
+      <c r="J4">
         <v>17</v>
       </c>
-      <c r="I4" s="2">
-        <f t="shared" si="1"/>
+      <c r="K4" s="2">
+        <f t="shared" si="3"/>
         <v>11.038961038961039</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>1</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M4">
+      <c r="M4" s="2">
+        <f t="shared" si="4"/>
+        <v>9.0991810737033677E-2</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P4">
         <v>135</v>
       </c>
-      <c r="N4">
+      <c r="Q4" s="2">
+        <f t="shared" si="6"/>
+        <v>9.9778270509977833</v>
+      </c>
+      <c r="R4">
         <v>134</v>
       </c>
-      <c r="O4" s="2">
-        <f t="shared" si="3"/>
+      <c r="S4" s="2">
+        <f t="shared" si="7"/>
         <v>87.012987012987011</v>
       </c>
-      <c r="P4">
+      <c r="T4">
         <v>3</v>
       </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="U4" s="2">
+        <f t="shared" si="8"/>
+        <v>0.22455089820359281</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1392,55 +1478,75 @@
       <c r="D5">
         <v>239</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>7.9008264462809921</v>
+      </c>
+      <c r="F5">
         <v>101</v>
       </c>
-      <c r="F5" s="2">
-        <f t="shared" si="0"/>
+      <c r="G5" s="2">
+        <f t="shared" si="1"/>
         <v>25.062034739454091</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>217</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
       <c r="I5" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>5.1642075202284632</v>
       </c>
       <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L5">
         <v>171</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M5">
+      <c r="M5" s="2">
+        <f t="shared" si="4"/>
+        <v>15.559599636032756</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P5">
         <v>287</v>
       </c>
-      <c r="N5">
+      <c r="Q5" s="2">
+        <f t="shared" si="6"/>
+        <v>21.212121212121211</v>
+      </c>
+      <c r="R5">
         <v>51</v>
       </c>
-      <c r="O5" s="2">
-        <f t="shared" si="3"/>
+      <c r="S5" s="2">
+        <f t="shared" si="7"/>
         <v>12.655086848635236</v>
       </c>
-      <c r="P5">
+      <c r="T5">
         <v>197</v>
       </c>
-      <c r="Q5">
+      <c r="U5" s="2">
+        <f t="shared" si="8"/>
+        <v>14.745508982035929</v>
+      </c>
+      <c r="V5">
         <v>3</v>
       </c>
-      <c r="R5" s="2">
-        <f t="shared" si="4"/>
+      <c r="W5" s="2">
+        <f t="shared" si="9"/>
         <v>0.74441687344913154</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1453,1178 +1559,1613 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="E6" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G6">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>3</v>
+      </c>
+      <c r="U6" s="2">
+        <f t="shared" si="8"/>
+        <v>0.22455089820359281</v>
+      </c>
+      <c r="V6">
+        <v>3</v>
+      </c>
+      <c r="W6" s="2">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7">
+        <v>299</v>
+      </c>
+      <c r="C7">
+        <v>35</v>
+      </c>
+      <c r="D7">
+        <v>48</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5867768595041323</v>
+      </c>
+      <c r="F7">
+        <v>9</v>
+      </c>
+      <c r="G7" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2">
+        <v>3.0100334448160537</v>
+      </c>
+      <c r="H7">
+        <v>277</v>
+      </c>
+      <c r="I7" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6" s="2">
+        <v>6.5920990004759634</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P6">
+        <v>1.3377926421404682</v>
+      </c>
+      <c r="L7">
+        <v>262</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="4"/>
+        <v>23.83985441310282</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>245</v>
+      </c>
+      <c r="Q7" s="2">
+        <f t="shared" si="6"/>
+        <v>18.107908351810792</v>
+      </c>
+      <c r="R7">
+        <v>6</v>
+      </c>
+      <c r="S7" s="2">
+        <f t="shared" si="7"/>
+        <v>2.0066889632107023</v>
+      </c>
+      <c r="T7">
+        <v>272</v>
+      </c>
+      <c r="U7" s="2">
+        <f t="shared" si="8"/>
+        <v>20.359281437125748</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>11</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="2"/>
+        <v>0.26178010471204188</v>
+      </c>
+      <c r="J8">
+        <v>11</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9">
+        <v>53</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>46</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0947168015230844</v>
+      </c>
+      <c r="J9">
         <v>3</v>
       </c>
-      <c r="Q6">
+      <c r="K9" s="2">
+        <f t="shared" si="3"/>
+        <v>5.6603773584905666</v>
+      </c>
+      <c r="L9">
+        <v>40</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="4"/>
+        <v>3.6396724294813465</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>40</v>
+      </c>
+      <c r="Q9" s="2">
+        <f t="shared" si="6"/>
+        <v>2.9563932002956395</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>50</v>
+      </c>
+      <c r="U9" s="2">
+        <f t="shared" si="8"/>
+        <v>3.7425149700598799</v>
+      </c>
+      <c r="V9">
+        <v>5</v>
+      </c>
+      <c r="W9" s="2">
+        <f t="shared" si="9"/>
+        <v>9.433962264150944</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="2"/>
+        <v>4.7596382674916705E-2</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="4"/>
+        <v>0.18198362147406735</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="2">
+        <f t="shared" si="6"/>
+        <v>0.14781966001478197</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10" s="2">
+        <f t="shared" si="8"/>
+        <v>7.4850299401197612E-2</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>1354</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1200</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>39.669421487603309</v>
+      </c>
+      <c r="F11">
+        <v>1191</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="1"/>
+        <v>87.961595273264408</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>163</v>
+      </c>
+      <c r="U11" s="2">
+        <f t="shared" si="8"/>
+        <v>12.200598802395209</v>
+      </c>
+      <c r="V11">
+        <v>154</v>
+      </c>
+      <c r="W11" s="2">
+        <f t="shared" si="9"/>
+        <v>11.37370753323486</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12">
+        <v>742</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>3.3057851239669422E-2</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>710</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="2"/>
+        <v>16.896715849595431</v>
+      </c>
+      <c r="J12">
+        <v>515</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="3"/>
+        <v>69.40700808625337</v>
+      </c>
+      <c r="L12">
+        <v>210</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="4"/>
+        <v>19.108280254777071</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12" s="2">
+        <f t="shared" si="5"/>
+        <v>0.13477088948787064</v>
+      </c>
+      <c r="P12">
+        <v>205</v>
+      </c>
+      <c r="Q12" s="2">
+        <f t="shared" si="6"/>
+        <v>15.151515151515152</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12" s="2">
+        <f t="shared" si="7"/>
+        <v>0.13477088948787064</v>
+      </c>
+      <c r="T12">
+        <v>220</v>
+      </c>
+      <c r="U12" s="2">
+        <f t="shared" si="8"/>
+        <v>16.467065868263472</v>
+      </c>
+      <c r="V12">
+        <v>7</v>
+      </c>
+      <c r="W12" s="2">
+        <f t="shared" si="9"/>
+        <v>0.94339622641509435</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>8</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="2"/>
+        <v>0.19038553069966682</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>4</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="4"/>
+        <v>0.36396724294813471</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P13">
         <v>3</v>
       </c>
-      <c r="R6" s="2">
+      <c r="Q13" s="2">
+        <f t="shared" si="6"/>
+        <v>0.22172949002217296</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>9</v>
+      </c>
+      <c r="U13" s="2">
+        <f t="shared" si="8"/>
+        <v>0.67365269461077848</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>1707</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>1657</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="2"/>
+        <v>39.433603046168493</v>
+      </c>
+      <c r="J14">
+        <v>1596</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" si="3"/>
+        <v>93.49736379613357</v>
+      </c>
+      <c r="L14">
+        <v>110</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="4"/>
+        <v>10.009099181073704</v>
+      </c>
+      <c r="N14">
+        <v>13</v>
+      </c>
+      <c r="O14" s="2">
+        <f t="shared" si="5"/>
+        <v>0.76157000585823076</v>
+      </c>
+      <c r="P14">
+        <v>88</v>
+      </c>
+      <c r="Q14" s="2">
+        <f t="shared" si="6"/>
+        <v>6.5040650406504072</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>89</v>
+      </c>
+      <c r="U14" s="2">
+        <f t="shared" si="8"/>
+        <v>6.6616766467065869</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14" s="2">
+        <f t="shared" si="9"/>
+        <v>5.8582308142940832E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15">
+        <v>69</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>68</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="2"/>
+        <v>1.618277010947168</v>
+      </c>
+      <c r="J15">
+        <v>68</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="3"/>
+        <v>98.550724637681171</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15" s="2">
+        <f t="shared" si="8"/>
+        <v>7.4850299401197612E-2</v>
+      </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
+      <c r="W15" s="2">
+        <f t="shared" si="9"/>
+        <v>1.4492753623188406</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16">
+        <v>97</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>76</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="2"/>
+        <v>1.8086625416468347</v>
+      </c>
+      <c r="J16">
+        <v>76</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="3"/>
+        <v>78.350515463917532</v>
+      </c>
+      <c r="L16">
+        <v>20</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="4"/>
+        <v>1.8198362147406733</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>20</v>
+      </c>
+      <c r="Q16" s="2">
+        <f t="shared" si="6"/>
+        <v>1.4781966001478197</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>20</v>
+      </c>
+      <c r="U16" s="2">
+        <f t="shared" si="8"/>
+        <v>1.4970059880239521</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>6</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="2"/>
+        <v>0.14278914802475012</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>6</v>
+      </c>
+      <c r="Q17" s="2">
+        <f t="shared" si="6"/>
+        <v>0.44345898004434592</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18">
+        <v>155</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>154</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="2"/>
+        <v>3.664921465968586</v>
+      </c>
+      <c r="J18">
+        <v>149</v>
+      </c>
+      <c r="K18" s="2">
+        <f t="shared" si="3"/>
+        <v>96.129032258064512</v>
+      </c>
+      <c r="L18">
+        <v>5</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="4"/>
+        <v>0.45495905368516831</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>5</v>
+      </c>
+      <c r="Q18" s="2">
+        <f t="shared" si="6"/>
+        <v>0.36954915003695493</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>6</v>
+      </c>
+      <c r="U18" s="2">
+        <f t="shared" si="8"/>
+        <v>0.44910179640718562</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="W18" s="2">
+        <f t="shared" si="9"/>
+        <v>0.64516129032258063</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19">
+        <v>205</v>
+      </c>
+      <c r="C19">
+        <v>84</v>
+      </c>
+      <c r="D19">
+        <v>182</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>6.0165289256198342</v>
+      </c>
+      <c r="F19">
+        <v>95</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>46.341463414634148</v>
+      </c>
+      <c r="H19">
+        <v>106</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="2"/>
+        <v>2.5226082817705855</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>106</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" si="4"/>
+        <v>9.6451319381255693</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19" s="2">
+        <f t="shared" si="5"/>
+        <v>0.48780487804878048</v>
+      </c>
+      <c r="P19">
+        <v>109</v>
+      </c>
+      <c r="Q19" s="2">
+        <f t="shared" si="6"/>
+        <v>8.0561714708056176</v>
+      </c>
+      <c r="R19">
+        <v>2</v>
+      </c>
+      <c r="S19" s="2">
+        <f t="shared" si="7"/>
+        <v>0.97560975609756095</v>
+      </c>
+      <c r="T19">
+        <v>94</v>
+      </c>
+      <c r="U19" s="2">
+        <f t="shared" si="8"/>
+        <v>7.0359281437125745</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20">
+        <v>399</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.26446280991735538</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>399</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="2"/>
+        <v>9.4954783436458836</v>
+      </c>
+      <c r="J20">
+        <v>375</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" si="3"/>
+        <v>93.984962406015043</v>
+      </c>
+      <c r="L20">
+        <v>21</v>
+      </c>
+      <c r="M20" s="2">
+        <f t="shared" si="4"/>
+        <v>1.910828025477707</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>20</v>
+      </c>
+      <c r="Q20" s="2">
+        <f t="shared" si="6"/>
+        <v>1.4781966001478197</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>20</v>
+      </c>
+      <c r="U20" s="2">
+        <f t="shared" si="8"/>
+        <v>1.4970059880239521</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21">
+        <v>69</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>69</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="2"/>
+        <v>1.6420752022846263</v>
+      </c>
+      <c r="J21">
+        <v>57</v>
+      </c>
+      <c r="K21" s="2">
+        <f t="shared" si="3"/>
+        <v>82.608695652173907</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21" s="2">
+        <f t="shared" si="4"/>
+        <v>9.0991810737033677E-2</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>10</v>
+      </c>
+      <c r="Q21" s="2">
+        <f t="shared" si="6"/>
+        <v>0.73909830007390986</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>12</v>
+      </c>
+      <c r="U21" s="2">
+        <f t="shared" si="8"/>
+        <v>0.89820359281437123</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>2</v>
+      </c>
+      <c r="M22" s="2">
+        <f t="shared" si="4"/>
+        <v>0.18198362147406735</v>
+      </c>
+      <c r="N22">
+        <v>2</v>
+      </c>
+      <c r="O22" s="2">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>8</v>
+      </c>
+      <c r="U22" s="2">
+        <f t="shared" si="8"/>
+        <v>0.5988023952095809</v>
+      </c>
+      <c r="V22">
+        <v>8</v>
+      </c>
+      <c r="W22" s="2">
+        <f t="shared" si="9"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>1208</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>1187</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="0"/>
+        <v>39.239669421487605</v>
+      </c>
+      <c r="F23">
+        <v>1178</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="1"/>
+        <v>97.516556291390728</v>
+      </c>
+      <c r="H23">
+        <v>27</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="2"/>
+        <v>0.64255116611137553</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>21</v>
+      </c>
+      <c r="M23" s="2">
+        <f t="shared" si="4"/>
+        <v>1.910828025477707</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>29</v>
+      </c>
+      <c r="Q23" s="2">
+        <f t="shared" si="6"/>
+        <v>2.1433850702143387</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>29</v>
+      </c>
+      <c r="U23" s="2">
+        <f t="shared" si="8"/>
+        <v>2.1706586826347305</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24">
+        <v>7478</v>
+      </c>
+      <c r="C24">
+        <v>257</v>
+      </c>
+      <c r="D24">
+        <v>3025</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F24">
+        <v>2695</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="1"/>
+        <v>36.039047873763039</v>
+      </c>
+      <c r="H24">
+        <v>4202</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="J24">
+        <v>3098</v>
+      </c>
+      <c r="K24" s="2">
+        <f t="shared" si="3"/>
+        <v>41.428189355442626</v>
+      </c>
+      <c r="L24">
+        <v>1099</v>
+      </c>
+      <c r="M24" s="2">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7">
-        <v>299</v>
-      </c>
-      <c r="C7">
-        <v>35</v>
-      </c>
-      <c r="D7">
-        <v>48</v>
-      </c>
-      <c r="E7">
-        <v>9</v>
-      </c>
-      <c r="F7" s="2">
-        <f t="shared" si="0"/>
-        <v>3.0100334448160537</v>
-      </c>
-      <c r="G7">
-        <v>277</v>
-      </c>
-      <c r="H7">
-        <v>4</v>
-      </c>
-      <c r="I7" s="2">
-        <f t="shared" si="1"/>
-        <v>1.3377926421404682</v>
-      </c>
-      <c r="J7">
-        <v>262</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>245</v>
-      </c>
-      <c r="N7">
-        <v>6</v>
-      </c>
-      <c r="O7" s="2">
-        <f t="shared" si="3"/>
-        <v>2.0066889632107023</v>
-      </c>
-      <c r="P7">
-        <v>272</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8">
-        <v>11</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>11</v>
-      </c>
-      <c r="H8">
-        <v>11</v>
-      </c>
-      <c r="I8" s="2">
-        <f t="shared" si="1"/>
+      <c r="N24">
+        <v>17</v>
+      </c>
+      <c r="O24" s="2">
+        <f t="shared" si="5"/>
+        <v>0.22733351163412679</v>
+      </c>
+      <c r="P24">
+        <v>1353</v>
+      </c>
+      <c r="Q24" s="2">
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9">
-        <v>53</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>46</v>
-      </c>
-      <c r="H9">
-        <v>3</v>
-      </c>
-      <c r="I9" s="2">
-        <f t="shared" si="1"/>
-        <v>5.6603773584905666</v>
-      </c>
-      <c r="J9">
-        <v>40</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>40</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>50</v>
-      </c>
-      <c r="Q9">
-        <v>5</v>
-      </c>
-      <c r="R9" s="2">
-        <f t="shared" si="4"/>
-        <v>9.433962264150944</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>2</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>2</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>2</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>1</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11">
-        <v>1354</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>1200</v>
-      </c>
-      <c r="E11">
-        <v>1191</v>
-      </c>
-      <c r="F11" s="2">
-        <f t="shared" si="0"/>
-        <v>87.961595273264408</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>163</v>
-      </c>
-      <c r="Q11">
-        <v>154</v>
-      </c>
-      <c r="R11" s="2">
-        <f t="shared" si="4"/>
-        <v>11.37370753323486</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12">
-        <v>742</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>710</v>
-      </c>
-      <c r="H12">
-        <v>515</v>
-      </c>
-      <c r="I12" s="2">
-        <f t="shared" si="1"/>
-        <v>69.40700808625337</v>
-      </c>
-      <c r="J12">
-        <v>210</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12" s="2">
-        <f t="shared" si="2"/>
-        <v>0.13477088948787064</v>
-      </c>
-      <c r="M12">
-        <v>205</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-      <c r="O12" s="2">
-        <f t="shared" si="3"/>
-        <v>0.13477088948787064</v>
-      </c>
-      <c r="P12">
-        <v>220</v>
-      </c>
-      <c r="Q12">
-        <v>7</v>
-      </c>
-      <c r="R12" s="2">
-        <f t="shared" si="4"/>
-        <v>0.94339622641509435</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13">
-        <v>10</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>8</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>4</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>3</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>9</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14">
-        <v>1707</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>1657</v>
-      </c>
-      <c r="H14">
-        <v>1596</v>
-      </c>
-      <c r="I14" s="2">
-        <f t="shared" si="1"/>
-        <v>93.49736379613357</v>
-      </c>
-      <c r="J14">
-        <v>110</v>
-      </c>
-      <c r="K14">
-        <v>13</v>
-      </c>
-      <c r="L14" s="2">
-        <f t="shared" si="2"/>
-        <v>0.76157000585823076</v>
-      </c>
-      <c r="M14">
-        <v>88</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P14">
-        <v>89</v>
-      </c>
-      <c r="Q14">
-        <v>1</v>
-      </c>
-      <c r="R14" s="2">
-        <f t="shared" si="4"/>
-        <v>5.8582308142940832E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15">
-        <v>69</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>68</v>
-      </c>
-      <c r="H15">
-        <v>68</v>
-      </c>
-      <c r="I15" s="2">
-        <f t="shared" si="1"/>
-        <v>98.550724637681171</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>1</v>
-      </c>
-      <c r="Q15">
-        <v>1</v>
-      </c>
-      <c r="R15" s="2">
-        <f t="shared" si="4"/>
-        <v>1.4492753623188406</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16">
-        <v>97</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>76</v>
-      </c>
-      <c r="H16">
-        <v>76</v>
-      </c>
-      <c r="I16" s="2">
-        <f t="shared" si="1"/>
-        <v>78.350515463917532</v>
-      </c>
-      <c r="J16">
-        <v>20</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <v>20</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>20</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17">
-        <v>6</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>6</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>6</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18">
-        <v>155</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>154</v>
-      </c>
-      <c r="H18">
-        <v>149</v>
-      </c>
-      <c r="I18" s="2">
-        <f t="shared" si="1"/>
-        <v>96.129032258064512</v>
-      </c>
-      <c r="J18">
-        <v>5</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>5</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>6</v>
-      </c>
-      <c r="Q18">
-        <v>1</v>
-      </c>
-      <c r="R18" s="2">
-        <f t="shared" si="4"/>
-        <v>0.64516129032258063</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19">
-        <v>205</v>
-      </c>
-      <c r="C19">
-        <v>84</v>
-      </c>
-      <c r="D19">
-        <v>182</v>
-      </c>
-      <c r="E19">
-        <v>95</v>
-      </c>
-      <c r="F19" s="2">
-        <f t="shared" si="0"/>
-        <v>46.341463414634148</v>
-      </c>
-      <c r="G19">
-        <v>106</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>106</v>
-      </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
-      <c r="L19" s="2">
-        <f t="shared" si="2"/>
-        <v>0.48780487804878048</v>
-      </c>
-      <c r="M19">
-        <v>109</v>
-      </c>
-      <c r="N19">
-        <v>2</v>
-      </c>
-      <c r="O19" s="2">
-        <f t="shared" si="3"/>
-        <v>0.97560975609756095</v>
-      </c>
-      <c r="P19">
-        <v>94</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20">
-        <v>399</v>
-      </c>
-      <c r="C20">
-        <v>8</v>
-      </c>
-      <c r="D20">
-        <v>8</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>399</v>
-      </c>
-      <c r="H20">
-        <v>375</v>
-      </c>
-      <c r="I20" s="2">
-        <f t="shared" si="1"/>
-        <v>93.984962406015043</v>
-      </c>
-      <c r="J20">
-        <v>21</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>20</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P20">
-        <v>20</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21">
-        <v>69</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>69</v>
-      </c>
-      <c r="H21">
-        <v>57</v>
-      </c>
-      <c r="I21" s="2">
-        <f t="shared" si="1"/>
-        <v>82.608695652173907</v>
-      </c>
-      <c r="J21">
-        <v>1</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>10</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P21">
-        <v>12</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22">
-        <v>10</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>2</v>
-      </c>
-      <c r="K22">
-        <v>2</v>
-      </c>
-      <c r="L22" s="2">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="O22" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P22">
-        <v>8</v>
-      </c>
-      <c r="Q22">
-        <v>8</v>
-      </c>
-      <c r="R22" s="2">
-        <f t="shared" si="4"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23">
-        <v>1208</v>
-      </c>
-      <c r="C23">
-        <v>5</v>
-      </c>
-      <c r="D23">
-        <v>1187</v>
-      </c>
-      <c r="E23">
-        <v>1178</v>
-      </c>
-      <c r="F23" s="2">
-        <f t="shared" si="0"/>
-        <v>97.516556291390728</v>
-      </c>
-      <c r="G23">
-        <v>27</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>21</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>29</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P23">
-        <v>29</v>
-      </c>
-      <c r="Q23">
-        <v>0</v>
-      </c>
-      <c r="R23" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24">
-        <v>7478</v>
-      </c>
-      <c r="C24">
-        <v>257</v>
-      </c>
-      <c r="D24">
-        <v>3025</v>
-      </c>
-      <c r="E24">
-        <v>2695</v>
-      </c>
-      <c r="F24" s="2">
-        <f t="shared" si="0"/>
-        <v>36.039047873763039</v>
-      </c>
-      <c r="G24">
-        <v>4202</v>
-      </c>
-      <c r="H24">
-        <v>3098</v>
-      </c>
-      <c r="I24" s="2">
-        <f t="shared" si="1"/>
-        <v>41.428189355442626</v>
-      </c>
-      <c r="J24">
-        <v>1099</v>
-      </c>
-      <c r="K24">
-        <v>17</v>
-      </c>
-      <c r="L24" s="2">
-        <f t="shared" si="2"/>
-        <v>0.22733351163412679</v>
-      </c>
-      <c r="M24">
-        <v>1353</v>
-      </c>
-      <c r="N24">
+      <c r="R24">
         <v>216</v>
       </c>
-      <c r="O24" s="2">
-        <f t="shared" si="3"/>
+      <c r="S24" s="2">
+        <f t="shared" si="7"/>
         <v>2.888472853704199</v>
       </c>
-      <c r="P24">
+      <c r="T24">
         <v>1336</v>
       </c>
-      <c r="Q24">
+      <c r="U24" s="2">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="V24">
         <v>188</v>
       </c>
-      <c r="R24" s="2">
-        <f t="shared" si="4"/>
+      <c r="W24" s="2">
+        <f t="shared" si="9"/>
         <v>2.5140411874832842</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="D25" s="2">
         <f>D24/B24*100</f>
         <v>40.451992511366676</v>
       </c>
-      <c r="G25" s="2">
-        <f>G24/B24*100</f>
+      <c r="E25" s="2"/>
+      <c r="H25" s="2">
+        <f>H24/B24*100</f>
         <v>56.191495052152987</v>
       </c>
-      <c r="J25" s="2">
-        <f>J24/B24*100</f>
+      <c r="I25" s="2"/>
+      <c r="L25" s="2">
+        <f>L24/B24*100</f>
         <v>14.696442899170901</v>
       </c>
-      <c r="M25" s="2">
-        <f>M24/B24*100</f>
-        <v>18.093073014174912</v>
-      </c>
+      <c r="M25" s="2"/>
       <c r="P25" s="2">
         <f>P24/B24*100</f>
+        <v>18.093073014174912</v>
+      </c>
+      <c r="Q25" s="2"/>
+      <c r="T25" s="2">
+        <f>T24/B24*100</f>
         <v>17.865739502540787</v>
       </c>
+      <c r="U25" s="2"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A7479">
     <sortCondition ref="A2:A7479"/>
   </sortState>
+  <conditionalFormatting sqref="E2:E23">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I23">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M23">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q2:Q23">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U2:U23">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2633,8 +3174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{350032C2-A8BF-4A50-9DE2-EB9790FF87DC}">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4186,7 +4727,7 @@
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>